<commit_message>
Added some collision maps and warp to the inn
</commit_message>
<xml_diff>
--- a/Planning/Menus.xlsx
+++ b/Planning/Menus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C86827F-F033-470E-9FF8-09C070C1ED26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32743F9-031A-43B0-A93C-4844A701A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="46770" yWindow="5100" windowWidth="28800" windowHeight="15435" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
@@ -2698,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A56A5F7-2FBC-4A35-A9C1-2015521BEBEF}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F35" sqref="F35:F42"/>
     </sheetView>
   </sheetViews>
@@ -4416,8 +4416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF75A49-A9C3-4B7E-8E19-E6842D7A7CB4}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,24 +4472,24 @@
         <v>69</v>
       </c>
       <c r="B2" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D2" s="14">
-        <v>2570</v>
+        <v>3904</v>
       </c>
       <c r="E2" s="14">
-        <v>7514</v>
+        <v>5188</v>
       </c>
       <c r="F2" s="6">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>266</v>
+        <v>64</v>
       </c>
       <c r="G2" s="6">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>64</v>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="L2" s="1" t="str">
         <f>_xlfn.CONCAT(A2,J2,H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>Shrine_Earth_Outside:{TileX:6,TileY:31,PlayerX:266,PlayerY:74},</v>
+        <v>Shrine_Earth_Outside:{TileX:10,TileY:21,PlayerX:64,PlayerY:148},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zelda can now die and respawn
</commit_message>
<xml_diff>
--- a/Planning/Menus.xlsx
+++ b/Planning/Menus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32743F9-031A-43B0-A93C-4844A701A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234C32D-FA47-48F1-8A0E-918417E944CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
+    <workbookView xWindow="47115" yWindow="5445" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
@@ -4417,7 +4417,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,24 +4472,24 @@
         <v>69</v>
       </c>
       <c r="B2" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D2" s="14">
-        <v>3904</v>
+        <v>4696</v>
       </c>
       <c r="E2" s="14">
-        <v>5188</v>
+        <v>7572</v>
       </c>
       <c r="F2" s="6">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="G2" s="6">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>64</v>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="L2" s="1" t="str">
         <f>_xlfn.CONCAT(A2,J2,H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>Shrine_Earth_Outside:{TileX:10,TileY:21,PlayerX:64,PlayerY:148},</v>
+        <v>Shrine_Earth_Outside:{TileX:12,TileY:31,PlayerX:88,PlayerY:132},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Shrine of Earth progress
</commit_message>
<xml_diff>
--- a/Planning/Menus.xlsx
+++ b/Planning/Menus.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234C32D-FA47-48F1-8A0E-918417E944CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A309C1CF-67CF-474D-AEEB-14D0E36D0F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47115" yWindow="5445" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{DF5BDE45-B0CE-4D37-9904-0D0A618A5DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
     <sheet name="Variables &amp; Scripts" sheetId="2" r:id="rId2"/>
-    <sheet name="OffsetCalculator" sheetId="3" r:id="rId3"/>
-    <sheet name="Items" sheetId="5" r:id="rId4"/>
+    <sheet name="Items" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="320">
   <si>
     <t>"Settings"</t>
   </si>
@@ -293,58 +292,7 @@
     <t>CurrentLocation</t>
   </si>
   <si>
-    <t>TileX</t>
-  </si>
-  <si>
-    <t>TileY</t>
-  </si>
-  <si>
-    <t>PlayerX</t>
-  </si>
-  <si>
-    <t>PlayerY</t>
-  </si>
-  <si>
-    <t>RealX</t>
-  </si>
-  <si>
-    <t>RealY</t>
-  </si>
-  <si>
-    <t>Tile Width</t>
-  </si>
-  <si>
-    <t>Tile Height</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>}</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>{</t>
-  </si>
-  <si>
-    <t>Is</t>
-  </si>
-  <si>
-    <t>Divider</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t>Shrine_Earth_Outside</t>
   </si>
   <si>
     <t>array_create(0)</t>
@@ -2112,7 +2060,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2144,13 +2092,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2202,7 +2143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2242,12 +2183,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2296,9 +2231,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2333,46 +2268,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2723,7 +2646,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2745,10 +2668,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2762,7 +2685,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -2779,7 +2702,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
@@ -2796,7 +2719,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E5" s="6">
         <v>2</v>
@@ -2843,16 +2766,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2868,7 +2791,7 @@
     </row>
     <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2890,30 +2813,30 @@
         <v>31</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2924,16 +2847,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D14" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2944,16 +2867,16 @@
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>16</v>
@@ -2969,16 +2892,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>7</v>
@@ -2988,7 +2911,7 @@
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -3015,13 +2938,13 @@
         <v>31</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="9" t="s">
@@ -3045,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="19" t="s">
         <v>40</v>
       </c>
       <c r="J19" s="3"/>
@@ -3053,16 +2976,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B20" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="F20" s="6">
         <v>3</v>
@@ -3076,16 +2999,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -3105,7 +3028,7 @@
         <v>27</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="F22" s="6">
         <v>1</v>
@@ -3118,7 +3041,7 @@
       <c r="A23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -3143,23 +3066,23 @@
         <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="G24" s="6" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="I24" s="3"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3184,13 +3107,13 @@
         <v>31</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="I26" s="3"/>
       <c r="M26" s="1"/>
@@ -3203,7 +3126,7 @@
         <v>41</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>46</v>
@@ -3226,7 +3149,7 @@
         <v>41</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>46</v>
@@ -3249,7 +3172,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>46</v>
@@ -3272,7 +3195,7 @@
         <v>41</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>46</v>
@@ -3295,23 +3218,23 @@
         <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="G31" s="6" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="I31" s="3"/>
       <c r="M31" s="1"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3336,29 +3259,29 @@
         <v>31</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="I33" s="3"/>
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="F34" s="6">
         <v>0</v>
@@ -3367,129 +3290,129 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>313</v>
+        <v>288</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C35" s="6" t="str">
         <f>_xlfn.CONCAT("SetInput(",A35,",arg0,global.CurrentConfigDevice)")</f>
         <v>SetInput("Left",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>313</v>
+        <v>289</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C36" s="6" t="str">
         <f t="shared" ref="C36:C42" si="0">_xlfn.CONCAT("SetInput(",A36,",arg0,global.CurrentConfigDevice)")</f>
         <v>SetInput("Right",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>313</v>
+        <v>290</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Up",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>313</v>
+        <v>291</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Down",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>313</v>
+        <v>292</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Action",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B40" s="24" t="s">
-        <v>313</v>
+        <v>293</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Special",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>313</v>
+        <v>294</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Inventory",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>313</v>
+        <v>295</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SetInput("Menu",arg0,global.CurrentConfigDevice)</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="G42" s="6"/>
     </row>
@@ -3501,13 +3424,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3700,7 +3623,7 @@
       <c r="G106" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3728,30 +3651,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -3764,18 +3687,18 @@
         <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1">
         <v>8</v>
@@ -3793,13 +3716,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -3812,18 +3735,18 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -3841,16 +3764,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3865,16 +3788,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3889,16 +3812,16 @@
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3913,13 +3836,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -3931,16 +3854,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>_xlfn.CONCAT(A10,B10," = ",D10,";")</f>
@@ -3949,16 +3872,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>_xlfn.CONCAT(A11,B11," = ",D11,";")</f>
@@ -3967,16 +3890,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>_xlfn.CONCAT(A12,B12," = ",D12,";")</f>
@@ -3985,16 +3908,16 @@
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="E13" s="3" t="str">
         <f>_xlfn.CONCAT(A13," ",B13," ",D13,";")</f>
@@ -4006,28 +3929,28 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1" t="str">
         <f t="shared" ref="E17:E22" si="1">_xlfn.CONCAT(A17,B17," = ",D17,";")</f>
@@ -4036,13 +3959,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
@@ -4054,13 +3977,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -4072,16 +3995,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4090,16 +4013,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4108,16 +4031,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4127,24 +4050,24 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>20</v>
@@ -4156,13 +4079,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1">
         <v>60</v>
@@ -4174,13 +4097,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D27" s="1">
         <v>60</v>
@@ -4192,13 +4115,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
@@ -4210,16 +4133,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="E29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4228,13 +4151,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -4246,16 +4169,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E31" s="1" t="str">
         <f>_xlfn.CONCAT(A31,B31," = ",D31,";")</f>
@@ -4264,16 +4187,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4282,16 +4205,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E33" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4300,16 +4223,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4318,16 +4241,16 @@
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E35" s="3" t="str">
         <f>_xlfn.CONCAT(A35,B35," = ",D35,";")</f>
@@ -4413,1087 +4336,970 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF75A49-A9C3-4B7E-8E19-E6842D7A7CB4}">
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="6">
-        <v>12</v>
-      </c>
-      <c r="C2" s="6">
-        <v>31</v>
-      </c>
-      <c r="D2" s="14">
-        <v>4696</v>
-      </c>
-      <c r="E2" s="14">
-        <v>7572</v>
-      </c>
-      <c r="F2" s="6">
-        <f>SUM(D2-B2*$B$4)</f>
-        <v>88</v>
-      </c>
-      <c r="G2" s="6">
-        <f>SUM(E2-C2*$B$5)</f>
-        <v>132</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f>_xlfn.CONCAT(A2,J2,H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>Shrine_Earth_Outside:{TileX:12,TileY:31,PlayerX:88,PlayerY:132},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="6">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="6">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E57697-7125-431C-8E9A-2A46B6506042}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="17"/>
-    <col min="2" max="2" width="40.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="17"/>
+    <col min="1" max="1" width="8.85546875" style="13"/>
+    <col min="2" max="2" width="40.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>12</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>14</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>20</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>21</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>22</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>23</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>24</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="18"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>26</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="18"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>27</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>28</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>29</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>30</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>31</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>32</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>33</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>34</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>35</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="18"/>
+    </row>
+    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>36</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>37</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>38</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="19" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>2</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>3</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>4</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>5</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>6</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>7</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>8</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>9</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>10</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>11</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>12</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>13</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="19" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>15</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <v>16</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
-        <v>17</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
-        <v>18</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
-        <v>19</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="E22" s="25"/>
-    </row>
-    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
-        <v>20</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="E23" s="25"/>
-    </row>
-    <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
-        <v>21</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="E24" s="25"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <v>22</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="22"/>
-    </row>
-    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
-        <v>23</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="19" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>24</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>270</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <v>25</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C28" s="22"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <v>26</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="22"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <v>27</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="19" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
-        <v>28</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="204.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
-        <v>29</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
-        <v>30</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
-        <v>31</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="22"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <v>32</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" s="22"/>
-    </row>
-    <row r="36" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>33</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>269</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
-        <v>34</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
-        <v>35</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C38" s="22"/>
-    </row>
-    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
-        <v>36</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
-        <v>37</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
-        <v>38</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="17" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D65" s="18"/>
-      <c r="E65" s="18"/>
-    </row>
-    <row r="66" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B66" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B67" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B68" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B70" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E5:E11"/>
     <mergeCell ref="E18:E24"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B75" r:id="rId1" location="Alligator_Shoes" xr:uid="{857E2DE7-8287-4040-995C-D2BFBB49E5B0}"/>
   </hyperlinks>

</xml_diff>